<commit_message>
Filled some more dates, types and remarks
</commit_message>
<xml_diff>
--- a/clariah-plus-workplan.xlsx
+++ b/clariah-plus-workplan.xlsx
@@ -28,32 +28,6 @@
     <author>p</author>
   </authors>
   <commentList>
-    <comment ref="C51" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Various components of this task would be more relevant for WP2, actually</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G28" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">But components date from over a decade before</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="I1" authorId="0">
       <text>
         <r>
@@ -63,7 +37,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">For software-related deliverables  I use the vocabulary of https://repostatus.org</t>
+          <t xml:space="preserve">Status for software deliverables uses the vocabulary from https://repostatus.org</t>
         </r>
       </text>
     </comment>
@@ -72,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="225">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -273,6 +247,9 @@
   </si>
   <si>
     <t xml:space="preserve">FoLiA v2.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q3 2018</t>
   </si>
   <si>
     <t xml:space="preserve">T108M2</t>
@@ -453,16 +430,22 @@
     <t xml:space="preserve">Deepfrog</t>
   </si>
   <si>
+    <t xml:space="preserve">(Q3 2020)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suspended</t>
   </si>
   <si>
-    <t xml:space="preserve">Jan 2021: The DeepFrog task is on hold as there seems to be no official budget/time for it and other priorities have taken precendence.</t>
+    <t xml:space="preserve">Jan 2021: The DeepFrog task is on hold since Q3 2020 as there seems to be no official budget/time for it and other priorities have taken precendence.</t>
   </si>
   <si>
     <t xml:space="preserve">T139bD1.1</t>
   </si>
   <si>
     <t xml:space="preserve">Deepfrog documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idem</t>
   </si>
   <si>
     <t xml:space="preserve">T139bD1.2</t>
@@ -634,6 +617,9 @@
     <t xml:space="preserve">Integration of webservice/webapp testing/monitoring facilities</t>
   </si>
   <si>
+    <t xml:space="preserve">postponed in favour of other priorities</t>
+  </si>
+  <si>
     <t xml:space="preserve">Authentication Milestone - LaMachine#171 -</t>
   </si>
   <si>
@@ -659,9 +645,6 @@
   </si>
   <si>
     <t xml:space="preserve">Q4 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2 2021?</t>
   </si>
   <si>
     <t xml:space="preserve">This is a development and coordination task</t>
@@ -692,6 +675,9 @@
   </si>
   <si>
     <t xml:space="preserve">Q3 2021?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">starts after completion of the most significant milestones</t>
   </si>
   <si>
     <t xml:space="preserve">T137M1</t>
@@ -929,7 +915,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1051,6 +1037,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1151,9 +1145,9 @@
   <dimension ref="A1:AD91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
+      <selection pane="bottomLeft" activeCell="I60" activeCellId="0" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1315,7 +1309,9 @@
       <c r="D5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" s="0" t="s">
         <v>30</v>
       </c>
@@ -1669,11 +1665,15 @@
       <c r="D17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="F17" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="H17" s="18" t="s">
         <v>17</v>
       </c>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="18" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>14</v>
@@ -1695,43 +1695,45 @@
       <c r="D18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="F18" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L18" s="23"/>
     </row>
     <row r="19" s="16" customFormat="true" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>17</v>
@@ -1746,7 +1748,7 @@
         <v>20</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L19" s="15" t="s">
         <v>22</v>
@@ -1758,7 +1760,7 @@
     <row r="20" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="27"/>
       <c r="B20" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>14</v>
@@ -1770,7 +1772,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G20" s="20" t="n">
         <v>2014</v>
@@ -1788,7 +1790,7 @@
     <row r="21" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="27"/>
       <c r="B21" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>14</v>
@@ -1800,9 +1802,11 @@
         <v>27</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="G21" s="20" t="n">
+        <v>2016</v>
+      </c>
       <c r="H21" s="21"/>
       <c r="I21" s="22" t="s">
         <v>25</v>
@@ -1816,7 +1820,7 @@
     <row r="22" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="27"/>
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>14</v>
@@ -1828,9 +1832,11 @@
         <v>27</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="21"/>
+        <v>82</v>
+      </c>
+      <c r="G22" s="20" t="n">
+        <v>2016</v>
+      </c>
       <c r="H22" s="21"/>
       <c r="I22" s="22" t="s">
         <v>25</v>
@@ -1844,7 +1850,7 @@
     <row r="23" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="27"/>
       <c r="B23" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>14</v>
@@ -1856,9 +1862,11 @@
         <v>27</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="21"/>
+        <v>84</v>
+      </c>
+      <c r="G23" s="20" t="n">
+        <v>2016</v>
+      </c>
       <c r="H23" s="21"/>
       <c r="I23" s="22" t="s">
         <v>25</v>
@@ -1872,7 +1880,7 @@
     <row r="24" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="27"/>
       <c r="B24" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>14</v>
@@ -1884,7 +1892,7 @@
         <v>15</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G24" s="20" t="n">
         <v>2015</v>
@@ -1902,7 +1910,7 @@
     <row r="25" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="27"/>
       <c r="B25" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>14</v>
@@ -1914,9 +1922,11 @@
         <v>62</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="21"/>
+        <v>88</v>
+      </c>
+      <c r="G25" s="20" t="n">
+        <v>2015</v>
+      </c>
       <c r="H25" s="21"/>
       <c r="I25" s="22" t="s">
         <v>25</v>
@@ -1930,7 +1940,7 @@
     <row r="26" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="27"/>
       <c r="B26" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>14</v>
@@ -1938,11 +1948,15 @@
       <c r="D26" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F26" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="21"/>
+        <v>90</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="H26" s="21" t="s">
         <v>60</v>
       </c>
@@ -1957,18 +1971,20 @@
     </row>
     <row r="27" s="16" customFormat="true" ht="44.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F27" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>17</v>
@@ -1977,13 +1993,13 @@
         <v>18</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>20</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L27" s="15" t="s">
         <v>22</v>
@@ -1991,22 +2007,22 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="G28" s="20" t="n">
         <v>2011</v>
@@ -2024,7 +2040,7 @@
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28"/>
       <c r="B29" s="24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>14</v>
@@ -2036,7 +2052,7 @@
         <v>27</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G29" s="20" t="n">
         <v>2018</v>
@@ -2054,7 +2070,7 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28"/>
       <c r="B30" s="24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>14</v>
@@ -2066,9 +2082,11 @@
         <v>41</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G30" s="21"/>
+        <v>101</v>
+      </c>
+      <c r="G30" s="20" t="n">
+        <v>2012</v>
+      </c>
       <c r="H30" s="21"/>
       <c r="I30" s="22" t="s">
         <v>25</v>
@@ -2082,7 +2100,7 @@
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28"/>
       <c r="B31" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>14</v>
@@ -2094,9 +2112,11 @@
         <v>15</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="21"/>
+        <v>103</v>
+      </c>
+      <c r="G31" s="20" t="n">
+        <v>2014</v>
+      </c>
       <c r="H31" s="21"/>
       <c r="I31" s="22" t="s">
         <v>25</v>
@@ -2110,7 +2130,7 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28"/>
       <c r="B32" s="24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>14</v>
@@ -2122,9 +2142,11 @@
         <v>15</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="G32" s="21"/>
+        <v>105</v>
+      </c>
+      <c r="G32" s="20" t="n">
+        <v>2012</v>
+      </c>
       <c r="H32" s="21"/>
       <c r="I32" s="22" t="s">
         <v>25</v>
@@ -2138,7 +2160,7 @@
     <row r="33" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="21"/>
       <c r="B33" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="18" t="s">
@@ -2148,11 +2170,13 @@
         <v>15</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G33" s="21"/>
+        <v>107</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>31</v>
+      </c>
       <c r="H33" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I33" s="22" t="s">
         <v>32</v>
@@ -2161,7 +2185,7 @@
         <v>20</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AD33" s="0" t="s">
         <v>32</v>
@@ -2170,7 +2194,7 @@
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28"/>
       <c r="B34" s="24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>14</v>
@@ -2182,7 +2206,7 @@
         <v>15</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G34" s="20" t="n">
         <v>2011</v>
@@ -2200,7 +2224,7 @@
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28"/>
       <c r="B35" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>14</v>
@@ -2212,9 +2236,11 @@
         <v>27</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="G35" s="21"/>
+        <v>113</v>
+      </c>
+      <c r="G35" s="20" t="n">
+        <v>2018</v>
+      </c>
       <c r="H35" s="21"/>
       <c r="I35" s="22" t="s">
         <v>25</v>
@@ -2228,7 +2254,7 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28"/>
       <c r="B36" s="24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>14</v>
@@ -2240,9 +2266,11 @@
         <v>41</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36" s="21"/>
+        <v>115</v>
+      </c>
+      <c r="G36" s="20" t="n">
+        <v>2016</v>
+      </c>
       <c r="H36" s="21"/>
       <c r="I36" s="22" t="s">
         <v>25</v>
@@ -2256,7 +2284,7 @@
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28"/>
       <c r="B37" s="24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>14</v>
@@ -2268,9 +2296,11 @@
         <v>15</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="21"/>
+        <v>117</v>
+      </c>
+      <c r="G37" s="20" t="n">
+        <v>2014</v>
+      </c>
       <c r="H37" s="21"/>
       <c r="I37" s="22" t="s">
         <v>25</v>
@@ -2284,7 +2314,7 @@
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28"/>
       <c r="B38" s="24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>14</v>
@@ -2296,9 +2326,11 @@
         <v>15</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="21"/>
+        <v>119</v>
+      </c>
+      <c r="G38" s="20" t="n">
+        <v>2012</v>
+      </c>
       <c r="H38" s="21"/>
       <c r="I38" s="22" t="s">
         <v>25</v>
@@ -2312,7 +2344,7 @@
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28"/>
       <c r="B39" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>14</v>
@@ -2324,9 +2356,11 @@
         <v>62</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G39" s="21"/>
+        <v>121</v>
+      </c>
+      <c r="G39" s="20" t="n">
+        <v>2012</v>
+      </c>
       <c r="H39" s="21"/>
       <c r="I39" s="22" t="s">
         <v>25</v>
@@ -2340,7 +2374,7 @@
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28"/>
       <c r="B40" s="24" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>14</v>
@@ -2352,9 +2386,11 @@
         <v>62</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="21"/>
+        <v>123</v>
+      </c>
+      <c r="G40" s="20" t="n">
+        <v>2012</v>
+      </c>
       <c r="H40" s="21"/>
       <c r="I40" s="22" t="s">
         <v>25</v>
@@ -2367,10 +2403,10 @@
     </row>
     <row r="41" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>14</v>
@@ -2382,24 +2418,28 @@
         <v>15</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
+        <v>126</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>127</v>
+      </c>
       <c r="I41" s="25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J41" s="18" t="s">
         <v>20</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="21"/>
       <c r="B42" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>14</v>
@@ -2411,22 +2451,28 @@
         <v>27</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
+        <v>131</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I42" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J42" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K42" s="19"/>
+      <c r="K42" s="19" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="21"/>
       <c r="B43" s="24" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>14</v>
@@ -2438,49 +2484,59 @@
         <v>15</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G43" s="21"/>
+        <v>134</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>108</v>
+      </c>
       <c r="H43" s="21"/>
       <c r="I43" s="25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J43" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K43" s="19"/>
+      <c r="K43" s="19" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="21"/>
       <c r="B44" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="I44" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K44" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J44" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K44" s="19"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="21"/>
       <c r="B45" s="24" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>14</v>
@@ -2492,22 +2548,26 @@
         <v>41</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G45" s="21"/>
+        <v>138</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>108</v>
+      </c>
       <c r="H45" s="21"/>
       <c r="I45" s="25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J45" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K45" s="19"/>
+      <c r="K45" s="19" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="21"/>
       <c r="B46" s="24" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>14</v>
@@ -2516,27 +2576,33 @@
         <v>24</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
+        <v>141</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I46" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J46" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K46" s="19"/>
+      <c r="K46" s="19" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>14</v>
@@ -2546,10 +2612,14 @@
       </c>
       <c r="E47" s="18"/>
       <c r="F47" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
+        <v>143</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="H47" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I47" s="22" t="s">
         <v>32</v>
       </c>
@@ -2563,10 +2633,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>14</v>
@@ -2574,31 +2644,37 @@
       <c r="D48" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="18"/>
+      <c r="E48" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="F48" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+        <v>145</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I48" s="25" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J48" s="18" t="s">
         <v>20</v>
       </c>
       <c r="K48" s="29" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="AD48" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>14</v>
@@ -2608,26 +2684,30 @@
       </c>
       <c r="E49" s="18"/>
       <c r="F49" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="I49" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="25" t="s">
-        <v>143</v>
-      </c>
       <c r="J49" s="18" t="s">
         <v>20</v>
       </c>
       <c r="AD49" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>14</v>
@@ -2637,12 +2717,16 @@
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
+        <v>151</v>
+      </c>
+      <c r="G50" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I50" s="25" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J50" s="18" t="s">
         <v>20</v>
@@ -2650,18 +2734,20 @@
     </row>
     <row r="51" s="16" customFormat="true" ht="44.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
+      <c r="E51" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F51" s="30" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G51" s="11" t="s">
         <v>17</v>
@@ -2676,21 +2762,21 @@
         <v>20</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="L51" s="15" t="s">
         <v>22</v>
       </c>
       <c r="AD51" s="16" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="18" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>14</v>
@@ -2702,7 +2788,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G52" s="20" t="n">
         <v>2015</v>
@@ -2721,7 +2807,7 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="18"/>
       <c r="B53" s="24" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>14</v>
@@ -2733,9 +2819,11 @@
         <v>27</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="G53" s="21"/>
+        <v>152</v>
+      </c>
+      <c r="G53" s="20" t="n">
+        <v>2015</v>
+      </c>
       <c r="H53" s="21"/>
       <c r="I53" s="22" t="s">
         <v>25</v>
@@ -2747,7 +2835,7 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="18"/>
       <c r="B54" s="24" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>14</v>
@@ -2756,12 +2844,14 @@
         <v>24</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="G54" s="21"/>
+        <v>161</v>
+      </c>
+      <c r="G54" s="20" t="n">
+        <v>2015</v>
+      </c>
       <c r="H54" s="21"/>
       <c r="I54" s="22" t="s">
         <v>25</v>
@@ -2771,23 +2861,25 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="18"/>
-      <c r="B55" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="G55" s="21"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="20" t="n">
+        <v>2018</v>
+      </c>
       <c r="H55" s="21"/>
       <c r="I55" s="22" t="s">
         <v>25</v>
@@ -2799,7 +2891,7 @@
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="18"/>
       <c r="B56" s="24" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>14</v>
@@ -2808,12 +2900,14 @@
         <v>24</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>163</v>
-      </c>
-      <c r="G56" s="21"/>
+        <v>166</v>
+      </c>
+      <c r="G56" s="20" t="n">
+        <v>2018</v>
+      </c>
       <c r="H56" s="21"/>
       <c r="I56" s="22" t="s">
         <v>25</v>
@@ -2824,10 +2918,10 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="18" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>14</v>
@@ -2839,7 +2933,7 @@
         <v>15</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G57" s="20" t="n">
         <v>2018</v>
@@ -2852,15 +2946,15 @@
         <v>20</v>
       </c>
       <c r="AD57" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="18" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>14</v>
@@ -2872,7 +2966,7 @@
         <v>15</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G58" s="20" t="n">
         <v>2018</v>
@@ -2885,15 +2979,15 @@
         <v>20</v>
       </c>
       <c r="AD58" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="18" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C59" s="17" t="s">
         <v>14</v>
@@ -2905,9 +2999,11 @@
         <v>15</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G59" s="21"/>
+        <v>177</v>
+      </c>
+      <c r="G59" s="20" t="n">
+        <v>2018</v>
+      </c>
       <c r="H59" s="21"/>
       <c r="I59" s="22" t="s">
         <v>25</v>
@@ -2916,15 +3012,15 @@
         <v>20</v>
       </c>
       <c r="AD59" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="18" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>14</v>
@@ -2933,12 +3029,14 @@
         <v>24</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="G60" s="21"/>
+        <v>182</v>
+      </c>
+      <c r="G60" s="20" t="n">
+        <v>2015</v>
+      </c>
       <c r="H60" s="21"/>
       <c r="I60" s="22" t="s">
         <v>25</v>
@@ -2949,10 +3047,10 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="18" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C61" s="17" t="s">
         <v>14</v>
@@ -2964,9 +3062,11 @@
         <v>15</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="G61" s="21"/>
+        <v>185</v>
+      </c>
+      <c r="G61" s="20" t="n">
+        <v>2016</v>
+      </c>
       <c r="H61" s="21"/>
       <c r="I61" s="22" t="s">
         <v>25</v>
@@ -2977,10 +3077,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>14</v>
@@ -2988,25 +3088,34 @@
       <c r="D62" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E62" s="21"/>
+      <c r="E62" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="F62" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
+        <v>188</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="I62" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J62" s="18" t="s">
         <v>20</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>14</v>
@@ -3014,17 +3123,19 @@
       <c r="D63" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E63" s="21"/>
+      <c r="E63" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="F63" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G63" s="21" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H63" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="I63" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="I63" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J63" s="18" t="s">
@@ -3032,25 +3143,27 @@
       </c>
     </row>
     <row r="64" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="B64" s="33" t="s">
-        <v>192</v>
+      <c r="A64" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>196</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="12"/>
-      <c r="E64" s="11"/>
+      <c r="E64" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="F64" s="30" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>195</v>
+        <v>70</v>
       </c>
       <c r="I64" s="14" t="s">
         <v>19</v>
@@ -3059,7 +3172,7 @@
         <v>20</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="L64" s="16" t="s">
         <v>22</v>
@@ -3067,10 +3180,10 @@
     </row>
     <row r="65" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C65" s="17" t="s">
         <v>14</v>
@@ -3082,15 +3195,15 @@
         <v>62</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="I65" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="I65" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J65" s="18" t="s">
@@ -3099,7 +3212,7 @@
     </row>
     <row r="66" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C66" s="17" t="s">
         <v>14</v>
@@ -3111,19 +3224,22 @@
         <v>27</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G66" s="21" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="I66" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J66" s="18" t="s">
         <v>20</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,7 +3247,7 @@
         <v>12</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C67" s="17" t="s">
         <v>14</v>
@@ -3139,15 +3255,17 @@
       <c r="D67" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E67" s="21"/>
+      <c r="E67" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="F67" s="19" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="G67" s="21"/>
       <c r="H67" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="I67" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="I67" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J67" s="18" t="s">
@@ -3156,10 +3274,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C68" s="17" t="s">
         <v>14</v>
@@ -3167,15 +3285,17 @@
       <c r="D68" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E68" s="21"/>
+      <c r="E68" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="F68" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G68" s="21"/>
       <c r="H68" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="I68" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="I68" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J68" s="18" t="s">
@@ -3184,10 +3304,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>14</v>
@@ -3195,15 +3315,17 @@
       <c r="D69" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E69" s="21"/>
+      <c r="E69" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="F69" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G69" s="21"/>
       <c r="H69" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="I69" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="I69" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J69" s="18" t="s">
@@ -3212,7 +3334,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>14</v>
@@ -3224,20 +3346,22 @@
         <v>41</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="G70" s="21"/>
+        <v>216</v>
+      </c>
+      <c r="G70" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="H70" s="21"/>
       <c r="I70" s="22" t="s">
         <v>25</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="24" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>14</v>
@@ -3249,10 +3373,10 @@
         <v>15</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G71" s="21" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H71" s="21"/>
       <c r="I71" s="22" t="s">
@@ -3264,26 +3388,28 @@
     </row>
     <row r="72" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="26" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="12"/>
-      <c r="E72" s="11"/>
+      <c r="E72" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="16"/>
       <c r="J72" s="11"/>
       <c r="K72" s="13" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="21" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="17"/>
@@ -3294,20 +3420,20 @@
         <v>15</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
       <c r="I73" s="25" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="J73" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="21" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="17"/>
@@ -3318,12 +3444,12 @@
         <v>15</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="G74" s="21"/>
       <c r="H74" s="21"/>
       <c r="I74" s="25" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="J74" s="21" t="s">
         <v>64</v>
@@ -3508,15 +3634,15 @@
       <c r="J90" s="21"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="34"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="34"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="34"/>
-      <c r="F91" s="34"/>
-      <c r="G91" s="34"/>
-      <c r="H91" s="34"/>
-      <c r="J91" s="34"/>
+      <c r="A91" s="36"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="36"/>
+      <c r="F91" s="36"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="36"/>
+      <c r="J91" s="36"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
set end date of VRE task to Q4 2021
</commit_message>
<xml_diff>
--- a/clariah-plus-workplan.xlsx
+++ b/clariah-plus-workplan.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="226">
   <si>
     <t xml:space="preserve">Project</t>
   </si>
@@ -661,10 +661,7 @@
 Extension of the current installation at CLST or a new one at HuC.</t>
   </si>
   <si>
-    <t xml:space="preserve">Q3 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q3 2021</t>
+    <t xml:space="preserve">Q4 2021</t>
   </si>
   <si>
     <t xml:space="preserve">T137D2</t>
@@ -674,7 +671,7 @@
 the form of screencast videos demonstrating various user stories.</t>
   </si>
   <si>
-    <t xml:space="preserve">Q3 2021?</t>
+    <t xml:space="preserve">Q3 2021</t>
   </si>
   <si>
     <t xml:space="preserve">starts after completion of the most significant milestones</t>
@@ -1153,7 +1150,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
+      <selection pane="bottomLeft" activeCell="H68" activeCellId="0" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3204,10 +3201,10 @@
         <v>202</v>
       </c>
       <c r="G65" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="H65" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="H65" s="21" t="s">
-        <v>204</v>
       </c>
       <c r="I65" s="33" t="s">
         <v>19</v>
@@ -3218,7 +3215,7 @@
     </row>
     <row r="66" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C66" s="17" t="s">
         <v>14</v>
@@ -3230,13 +3227,13 @@
         <v>27</v>
       </c>
       <c r="F66" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G66" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G66" s="21" t="s">
-        <v>194</v>
-      </c>
       <c r="H66" s="21" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I66" s="25" t="s">
         <v>71</v>
@@ -3245,7 +3242,7 @@
         <v>20</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,7 +3250,7 @@
         <v>12</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C67" s="17" t="s">
         <v>14</v>
@@ -3265,7 +3262,7 @@
         <v>15</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G67" s="21"/>
       <c r="H67" s="17" t="s">
@@ -3283,7 +3280,7 @@
         <v>73</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C68" s="17" t="s">
         <v>14</v>
@@ -3295,7 +3292,7 @@
         <v>15</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G68" s="21"/>
       <c r="H68" s="21" t="s">
@@ -3313,7 +3310,7 @@
         <v>152</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>14</v>
@@ -3325,7 +3322,7 @@
         <v>15</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G69" s="21"/>
       <c r="H69" s="21" t="s">
@@ -3340,7 +3337,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>14</v>
@@ -3352,7 +3349,7 @@
         <v>41</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G70" s="21" t="s">
         <v>17</v>
@@ -3362,24 +3359,24 @@
         <v>25</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="0" t="s">
         <v>218</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>219</v>
       </c>
       <c r="G71" s="21" t="s">
         <v>17</v>
@@ -3394,7 +3391,7 @@
     </row>
     <row r="72" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>70</v>
@@ -3410,12 +3407,12 @@
       <c r="I72" s="16"/>
       <c r="J72" s="11"/>
       <c r="K72" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="17"/>
@@ -3426,23 +3423,23 @@
         <v>15</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
       <c r="I73" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="J73" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="J73" s="21" t="s">
+      <c r="K73" s="0" t="s">
         <v>224</v>
-      </c>
-      <c r="K73" s="0" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="17"/>
@@ -3453,18 +3450,18 @@
         <v>15</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G74" s="21"/>
       <c r="H74" s="21"/>
       <c r="I74" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J74" s="21" t="s">
         <v>64</v>
       </c>
       <c r="K74" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>